<commit_message>
Monster + weapons update
</commit_message>
<xml_diff>
--- a/GameMasterGuide/Data/NewBeasts/beasts.xlsx
+++ b/GameMasterGuide/Data/NewBeasts/beasts.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$AI$158</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$AI$159</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="356">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -142,7 +142,9 @@
     <t xml:space="preserve">Acromantula</t>
   </si>
   <si>
-    <t xml:space="preserve">A newborn \imp{acromantula} has a shiny, hairless and pale-grey carapace, covering their body which is only 1 metre across, and has a diminished intelligence compared to their full grown counterparts. </t>
+    <t xml:space="preserve">A newborn \imp{acromantula} is tiny when compared to their full grown counterparts – though with a legspan of up to 40cm, they are still significantly larger than almost all non-magical spiders. 
+Their body is covered in a shiny, hairless and pale-grey carapace, which hardens and grows darker as they grow older – eventually they shed this skin as they enter the adult phase of their life. 
+Despite their limited intelligence and diluted poison, \name{}s are often encountered in nauseating flocks of thousands upon thousands, and in such large numbers, they pose a deadly threat to even the most powerful magic user. </t>
   </si>
   <si>
     <t xml:space="preserve">Non-Sapient</t>
@@ -176,7 +178,9 @@
     <t xml:space="preserve">Acromantula Adult</t>
   </si>
   <si>
-    <t xml:space="preserve">A fully grown \imp{Acromantula} is something to be greatly feared. They can run incredibly quickly and they utilise a ranged web attack to ensnare their pray, capturing it for later devourment….</t>
+    <t xml:space="preserve">From a nest of several thousand \imp{Hatchlings}, only one or two survive the brutal and vicious ascent to adulthood within an \imp{Acromantula} colony, shedding their final adolescant carapace to become a full-grown \imp{Acromantula}.
+As a result of this violent and competitive environment, a fully grown \imp{Acromantula} is something to be greatly feared. No \imp{Acromantula} survives this long without a willingness and ability to brutally slay even their closest allies, so that only the most murderous, brutal and cunning spiders remain. 
+Though  they can run incredibly quickly and they utilise a ranged web attack to ensnare their pray, the most terrifying aspect of a full-grown \imp{Acromantula} is their above-human level of intelligence, not only can they liquiefy your innards, they can counter even the most elaborate plan to outwit them. </t>
   </si>
   <si>
     <t xml:space="preserve">Sapient</t>
@@ -209,7 +213,9 @@
     <t xml:space="preserve">Acromantula Patriarch</t>
   </si>
   <si>
-    <t xml:space="preserve">The eldest of the spider monstrosities is known as the \imp{Patriarch}. Though they have reached truly gargantuan sizes, their bodies have become decrepit with age. Their minds, however, are razor sharp and they have mastered human speech. </t>
+    <t xml:space="preserve">If it is rare for a \imp{Hatchling} to survive to adulthood, it is even rarer for an \imp{Acromantula} to grow old, and gain the mantle of the \imp{Patriarch}. 
+As the \imp{Acromantula} never stop growing, by the time they reach 40 or 50 years old, they have reached truly gargantuan sizes, with legspans up to 10m, with an exoskeleton that is so thick that almost nothing can penetrate it. 
+Though they cut a truly terrifying figure, their bodies have become decrepit with age, and they do not retain the nimbleness of their younger forms, instead relying on their formidable intellect and their ability to command legions of their brood to protect them. </t>
   </si>
   <si>
     <t xml:space="preserve">\speaks{Human Languages, Spider Tongue}</t>
@@ -868,6 +874,37 @@
   </si>
   <si>
     <t xml:space="preserve">phlogiston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chalkydri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also known as the `Heralds of Dawn’, these winged serpent-like creatures were often mistaken for a species of \imp{Dragon} throughout history, and it is only recently that their true origins have been determined. 
+Possessing the face and tail of a crocodile, but the body of a lion and rows upon rows of wings (up to 12 pairs on the oldest known entities), these creatures reside within the coronosphere of a sun, descending planetside only for a few hours per year, and even then, they appear only during the first few moments of dawn. 
+When the sunlight hits their copper-bronze skin, it splits off into a mesmerising rainbow display, and causes their entire body to hum with a resonance like a chorus of angels. Legend holds that it is this song which brings the dawn, rather than the other way around.
+Though they do not seem particularly intelligent, and are currently classified as `beasts’ by the \imp{Ministry}, this does not mean that they are savage – in fact, the \name{} are often kind and gentle creatures, the few times that they have been recorded as coming into direct contact with humans it was eventually discovered that the humans were threatening some other life form with extinction, drawing the ire of the \name{}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incandescent, Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\melee{Reptilian Jaws}{10}{0}{Stabbing}{3 + Successes}
+\melee{Jagged Tail}{10}{2}{Bashing}{5 + Successes (Reach 5m)}
+\area{Downdraft}{circle 10m radius below current flying position)}{8}{0}{Prone}{1 + Successes}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\skill{Spellcasting}{7}
+\skill{Flight}{5}
+\skill{Regeneration}{4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\ability{Bringer of Dawn}{The \name{} may use its \imp{Spellcasting} ability to cast the \imp{Illuminate} spell.}
+\ability{Winged Herald}{The \name{} may use its \imp{Flight} skill to take to the skies, gaining a flying speed of 30m per round}
+\ability{Spectral Mesmer}{Any creature which comes within 20m and can see the \name{} must gain at least one success on a DV 8 check (recommended \imp{Willpower (Conviction)} to tear their eyes away from the hypnotising lights emanating from the \name{}, on a failure, they must spend their entire turn doing nothing but staring at the \name{}.}
+\ability{Light Siphon}{At the end of every round, if the \name{} can see a source of light, they regenerate health equal to a DV 4 \imp{Regeneration} check}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chalkydri</t>
   </si>
   <si>
     <t xml:space="preserve">Dugbog</t>
@@ -1288,12 +1325,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI158"/>
+  <dimension ref="A1:AI159"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Z105" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AH4" activeCellId="0" sqref="AH4"/>
+      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+      <selection pane="bottomLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
+      <selection pane="bottomRight" activeCell="AG108" activeCellId="0" sqref="AG108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1301,7 +1340,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="61.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="28" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="25.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="44.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.38"/>
@@ -1444,7 +1485,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="111.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -1533,7 +1574,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -1595,10 +1636,10 @@
         <v>1</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W4" s="1" t="n">
         <v>3</v>
@@ -1634,7 +1675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="111.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -4125,7 +4166,7 @@
         <v>4</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>153</v>
@@ -4200,35 +4241,111 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="6"/>
-      <c r="B107" s="7" t="s">
+    <row r="107" customFormat="false" ht="223.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D107" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D107" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E107" s="7" t="n">
+      <c r="E107" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K107" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F107" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G107" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH107" s="6"/>
+      <c r="L107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N107" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="O107" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P107" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q107" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T107" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="U107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="V107" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="W107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="X107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y107" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z107" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA107" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD107" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AE107" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF107" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG107" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH107" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI107" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="6"/>
       <c r="B108" s="7" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>98</v>
@@ -4247,16 +4364,16 @@
     <row r="109" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="6"/>
       <c r="B109" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>267</v>
+        <v>275</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>274</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E109" s="6" t="n">
-        <v>1</v>
+      <c r="E109" s="7" t="n">
+        <v>2</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>85</v>
@@ -4269,16 +4386,16 @@
     <row r="110" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6"/>
       <c r="B110" s="7" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E110" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>85</v>
@@ -4291,16 +4408,16 @@
     <row r="111" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6"/>
       <c r="B111" s="7" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E111" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>85</v>
@@ -4313,16 +4430,16 @@
     <row r="112" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6"/>
       <c r="B112" s="7" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E112" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>85</v>
@@ -4332,63 +4449,63 @@
       </c>
       <c r="AH112" s="6"/>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6"/>
       <c r="B113" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>273</v>
+        <v>279</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E113" s="7" t="n">
-        <v>6</v>
+      <c r="E113" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="AH113" s="6"/>
     </row>
-    <row r="114" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="6"/>
       <c r="B114" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>275</v>
+        <v>280</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E114" s="6" t="n">
-        <v>1</v>
+      <c r="E114" s="7" t="n">
+        <v>6</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="AH114" s="6"/>
     </row>
     <row r="115" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="6"/>
       <c r="B115" s="7" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E115" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F115" s="6" t="s">
         <v>85</v>
@@ -4398,19 +4515,19 @@
       </c>
       <c r="AH115" s="6"/>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="6"/>
       <c r="B116" s="7" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E116" s="6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>85</v>
@@ -4423,41 +4540,41 @@
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="6"/>
       <c r="B117" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>279</v>
+        <v>284</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E117" s="7" t="n">
-        <v>3</v>
+      <c r="E117" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="F117" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="AH117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="6"/>
       <c r="B118" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E118" s="6" t="n">
-        <v>4</v>
+      <c r="E118" s="7" t="n">
+        <v>3</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>195</v>
@@ -4467,10 +4584,10 @@
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="6"/>
       <c r="B119" s="7" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>98</v>
@@ -4479,7 +4596,7 @@
         <v>4</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>195</v>
@@ -4489,38 +4606,38 @@
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="6"/>
       <c r="B120" s="7" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E120" s="6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="AH120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="6"/>
       <c r="B121" s="7" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E121" s="6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F121" s="6" t="s">
         <v>85</v>
@@ -4533,59 +4650,59 @@
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="6"/>
       <c r="B122" s="7" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E122" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>41</v>
       </c>
       <c r="AH122" s="6"/>
     </row>
-    <row r="123" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="6"/>
       <c r="B123" s="7" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E123" s="6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="AH123" s="6"/>
     </row>
     <row r="124" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="6"/>
       <c r="B124" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>287</v>
+        <v>293</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E124" s="7" t="n">
+      <c r="E124" s="6" t="n">
         <v>2</v>
       </c>
       <c r="F124" s="6" t="s">
@@ -4599,16 +4716,16 @@
     <row r="125" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="6"/>
       <c r="B125" s="7" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E125" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>85</v>
@@ -4621,15 +4738,15 @@
     <row r="126" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="6"/>
       <c r="B126" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>287</v>
+        <v>296</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E126" s="6" t="n">
+      <c r="E126" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F126" s="6" t="s">
@@ -4640,41 +4757,41 @@
       </c>
       <c r="AH126" s="6"/>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="6"/>
       <c r="B127" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>292</v>
+        <v>297</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E127" s="7" t="n">
-        <v>4</v>
+      <c r="E127" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="AH127" s="6"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="6"/>
       <c r="B128" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>292</v>
+        <v>298</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>299</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E128" s="6" t="n">
-        <v>3</v>
+      <c r="E128" s="7" t="n">
+        <v>4</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>66</v>
@@ -4687,16 +4804,16 @@
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="6"/>
       <c r="B129" s="7" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E129" s="6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>66</v>
@@ -4709,38 +4826,38 @@
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="6"/>
       <c r="B130" s="7" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E130" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="AH130" s="6"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6"/>
       <c r="B131" s="7" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E131" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>85</v>
@@ -4753,54 +4870,54 @@
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="6"/>
       <c r="B132" s="7" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E132" s="6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="AH132" s="6"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="6"/>
       <c r="B133" s="7" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E133" s="6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>301</v>
+        <v>41</v>
       </c>
       <c r="AH133" s="6"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="6"/>
-      <c r="B134" s="6" t="s">
-        <v>302</v>
+      <c r="B134" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>98</v>
@@ -4812,39 +4929,39 @@
         <v>66</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="AH134" s="6"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="6"/>
-      <c r="B135" s="7" t="s">
-        <v>303</v>
+      <c r="B135" s="6" t="s">
+        <v>309</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E135" s="6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>99</v>
+        <v>308</v>
       </c>
       <c r="AH135" s="6"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="6"/>
       <c r="B136" s="7" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>98</v>
@@ -4853,20 +4970,20 @@
         <v>3</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="AH136" s="6"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="6"/>
       <c r="B137" s="7" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="D137" s="6" t="s">
         <v>98</v>
@@ -4885,15 +5002,15 @@
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6"/>
       <c r="B138" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>306</v>
+        <v>314</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E138" s="7" t="n">
+      <c r="E138" s="6" t="n">
         <v>3</v>
       </c>
       <c r="F138" s="6" t="s">
@@ -4907,16 +5024,16 @@
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="6"/>
       <c r="B139" s="7" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E139" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F139" s="6" t="s">
         <v>85</v>
@@ -4926,40 +5043,38 @@
       </c>
       <c r="AH139" s="6"/>
     </row>
-    <row r="140" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="6"/>
       <c r="B140" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>311</v>
+        <v>316</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>313</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E140" s="6" t="n">
-        <v>5</v>
+      <c r="E140" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="AH140" s="6"/>
     </row>
-    <row r="141" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="6" t="n">
-        <v>1</v>
-      </c>
+    <row r="141" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="6"/>
       <c r="B141" s="7" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>314</v>
+        <v>98</v>
       </c>
       <c r="E141" s="6" t="n">
         <v>5</v>
@@ -4968,30 +5083,25 @@
         <v>66</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH141" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="AI141" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="51.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>316</v>
+        <v>99</v>
+      </c>
+      <c r="AH141" s="6"/>
+    </row>
+    <row r="142" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E142" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F142" s="6" t="s">
         <v>66</v>
@@ -5000,21 +5110,24 @@
         <v>116</v>
       </c>
       <c r="AH142" s="6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>322</v>
+      </c>
+      <c r="AI142" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="51.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E143" s="6" t="n">
         <v>6</v>
@@ -5026,24 +5139,21 @@
         <v>116</v>
       </c>
       <c r="AH143" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="AI143" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="234.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="E144" s="6" t="n">
         <v>6</v>
@@ -5055,27 +5165,27 @@
         <v>116</v>
       </c>
       <c r="AH144" s="6" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="AI144" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="253.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="234.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="E145" s="6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F145" s="6" t="s">
         <v>66</v>
@@ -5084,41 +5194,48 @@
         <v>116</v>
       </c>
       <c r="AH145" s="6" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AI145" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="6"/>
-      <c r="B146" s="7" t="s">
-        <v>328</v>
+    <row r="146" customFormat="false" ht="253.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>332</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="E146" s="6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH146" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="AH146" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="AI146" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6"/>
       <c r="B147" s="7" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>98</v>
@@ -5130,70 +5247,70 @@
         <v>85</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>153</v>
+        <v>41</v>
       </c>
       <c r="AH147" s="6"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="6"/>
       <c r="B148" s="7" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E148" s="6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F148" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="AH148" s="6"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="6"/>
       <c r="B149" s="7" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E149" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="AH149" s="6"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="6"/>
       <c r="B150" s="7" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E150" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F150" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G150" s="6" t="s">
         <v>67</v>
@@ -5203,86 +5320,84 @@
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="6"/>
       <c r="B151" s="7" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E151" s="6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F151" s="6" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G151" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="AH151" s="6"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="6"/>
       <c r="B152" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>337</v>
+        <v>342</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E152" s="7" t="n">
-        <v>3</v>
+      <c r="E152" s="6" t="n">
+        <v>6</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G152" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH152" s="6" t="s">
-        <v>338</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="AH152" s="6"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="6"/>
       <c r="B153" s="7" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E153" s="7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="G153" s="6" t="s">
         <v>99</v>
       </c>
       <c r="AH153" s="6" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="6"/>
       <c r="B154" s="7" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E154" s="7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F154" s="6" t="s">
         <v>66</v>
@@ -5291,85 +5406,87 @@
         <v>99</v>
       </c>
       <c r="AH154" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="AI154" s="1" t="n">
-        <v>1</v>
+        <v>347</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="6"/>
-      <c r="B155" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C155" s="6" t="s">
+      <c r="B155" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C155" s="7" t="s">
         <v>344</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E155" s="6" t="n">
-        <v>4</v>
+      <c r="E155" s="7" t="n">
+        <v>5</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G155" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="AH155" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="AH155" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="AI155" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="6"/>
       <c r="B156" s="6" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E156" s="6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F156" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G156" s="6" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="AH156" s="6"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="6"/>
-      <c r="B157" s="7" t="s">
-        <v>346</v>
+      <c r="B157" s="6" t="s">
+        <v>352</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E157" s="6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F157" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G157" s="6" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="AH157" s="6"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="6"/>
       <c r="B158" s="7" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="D158" s="6" t="s">
         <v>98</v>
@@ -5385,8 +5502,30 @@
       </c>
       <c r="AH158" s="6"/>
     </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="6"/>
+      <c r="B159" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E159" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH159" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AI158"/>
+  <autoFilter ref="A2:AI159"/>
   <mergeCells count="8">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>